<commit_message>
upload updated notebooks and Output csv files
</commit_message>
<xml_diff>
--- a/flu_indicator/data/ML_models_on week40-20epiweek/ILI_weeks_testscores_allMLmodels.xlsx
+++ b/flu_indicator/data/ML_models_on week40-20epiweek/ILI_weeks_testscores_allMLmodels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emame\Desktop\FinalUCBX\flu_indicator\data\ML_models_on week40-20epiweek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B0F5CB-D9B9-4520-99E3-0CF5B7440C23}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7330B11A-562B-4431-8789-E63CEC1DFDAA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="14400" windowHeight="7360" xr2:uid="{39B0FB36-6A34-4C50-A98F-A2982686BAE6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{39B0FB36-6A34-4C50-A98F-A2982686BAE6}"/>
   </bookViews>
   <sheets>
     <sheet name="SUMMARY_STATS_ALL_FEATURES" sheetId="3" r:id="rId1"/>
@@ -34,9 +34,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t xml:space="preserve">kNN Regression </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SVM Regression </t>
   </si>
   <si>
     <t xml:space="preserve">Random Forest Regression  </t>
@@ -110,6 +107,9 @@
       </rPr>
       <t xml:space="preserve"> Mean Squared Error(MSE), Mean Absolute Error(MAE) by Machine learning models</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">SVM Regression </t>
   </si>
 </sst>
 </file>
@@ -583,7 +583,7 @@
   <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -598,31 +598,31 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9"/>
       <c r="B2" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="12"/>
       <c r="F2" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
       <c r="I2" s="12"/>
       <c r="J2" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
       <c r="M2" s="12"/>
       <c r="N2" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>
@@ -631,84 +631,84 @@
     <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="8"/>
       <c r="B3" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="F3" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="J3" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K3" s="14"/>
       <c r="L3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="N3" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O3" s="14"/>
       <c r="P3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="8"/>
       <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>8</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="6"/>
       <c r="F4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>8</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="6"/>
       <c r="J4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>8</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="6"/>
       <c r="N4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>8</v>
       </c>
       <c r="P4" s="4"/>
       <c r="Q4" s="6"/>
     </row>
     <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="7">
         <v>0.998</v>
@@ -761,7 +761,7 @@
     </row>
     <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="7">
         <v>0.90500000000000003</v>
@@ -788,10 +788,10 @@
         <v>0.316</v>
       </c>
       <c r="J6" s="7">
-        <v>0.85799999999999998</v>
+        <v>0.82699999999999996</v>
       </c>
       <c r="K6" s="7">
-        <v>0.58299999999999996</v>
+        <v>0.47699999999999998</v>
       </c>
       <c r="L6" s="7">
         <v>0.19800000000000001</v>
@@ -814,7 +814,7 @@
     </row>
     <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B7" s="7">
         <v>0.88100000000000001</v>
@@ -920,7 +920,7 @@
     </row>
     <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="7">
         <v>1</v>
@@ -970,6 +970,9 @@
       <c r="Q9" s="7">
         <v>0.93200000000000005</v>
       </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="J11" s="1"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="E14" s="1"/>

</xml_diff>